<commit_message>
Updated Bugs and Todos
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Last modified</t>
+  </si>
+  <si>
+    <t>View dispatch doesn't work</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>Jobs -&gt; Dispatches</t>
+  </si>
+  <si>
+    <t>The document created when pressing the "View dispatch" button is just a static sample document rather than content generated from the actual dispatch.</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +451,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>40245</v>
+      </c>
+      <c r="G2" s="5">
+        <v>40245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reworked SingerConstants class so that it can be used to pull parameters from the database instead of hard coded values.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>The document created when pressing the "View dispatch" button is just a static sample document rather than content generated from the actual dispatch.</t>
+  </si>
+  <si>
+    <t>Import loses customer type</t>
+  </si>
+  <si>
+    <t>Importer</t>
+  </si>
+  <si>
+    <t>The importing process does no mark what type of customer type each company is any more.</t>
   </si>
 </sst>
 </file>
@@ -56,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -104,10 +113,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +483,29 @@
         <v>40245</v>
       </c>
     </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>40245</v>
+      </c>
+      <c r="G3" s="5">
+        <v>40245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added bugs and todos and reorganized external programs and libraries.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>The importing process does no mark what type of customer type each company is any more.</t>
+  </si>
+  <si>
+    <t>Search crash in Edit Companies window</t>
+  </si>
+  <si>
+    <t>EditCompaniesWindow</t>
+  </si>
+  <si>
+    <t>Searching for a company that doesn’t exist will case a crash.</t>
+  </si>
+  <si>
+    <t>FIXED</t>
   </si>
 </sst>
 </file>
@@ -420,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +443,7 @@
     <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="5" customWidth="1"/>
@@ -503,6 +515,29 @@
         <v>40245</v>
       </c>
       <c r="G3" s="5">
+        <v>40245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5">
+        <v>40245</v>
+      </c>
+      <c r="G4" s="5">
         <v>40245</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved the document view button to a more global location for quotes and invoices.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve">After updating to the latest WPF Toolkit, the DatePicker controls all look disabled, even when they shouldn't be. </t>
+  </si>
+  <si>
+    <t>Images missing from PDF output</t>
+  </si>
+  <si>
+    <t>DocumentViewer</t>
+  </si>
+  <si>
+    <t>The wkhtmltopdf application seem to break images with a 'file://' url when converting to PDFs. This is likely a bug that I can't easily fix, so a workaround is needed.</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +462,7 @@
     <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="5" customWidth="1"/>
   </cols>
@@ -571,6 +580,29 @@
       </c>
       <c r="G5" s="5">
         <v>40246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5">
+        <v>40247</v>
+      </c>
+      <c r="G6" s="5">
+        <v>40247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Application is now targeting .NET 4.0 Client Profile.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -75,15 +75,9 @@
     <t>DatePicker controls look strange</t>
   </si>
   <si>
-    <t>WONTFIX</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>After updating to the latest WPF Toolkit, the DatePicker controls all look disabled, even when they shouldn't be.  (It appears that this is a bug with WPF Toolkit, so I will just wait until they fix it.)</t>
-  </si>
-  <si>
     <t>Images missing from PDF output</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>The wkhtmltopdf application seem to break images with a 'file://' url when converting to PDFs. This is likely a bug that I can't easily fix, so in the final version the required images will need to be placed on an HTTP server.</t>
+  </si>
+  <si>
+    <t>After updating to the latest WPF Toolkit, the DatePicker controls all look disabled, even when they shouldn't be.  Note1: It appears that this is a bug with WPF Toolkit, so I will just wait until they fix it.  Note2: I have fixed this issue by switching to the DataGrid and DatePicker controls in .net 4.0</t>
   </si>
 </sst>
 </file>
@@ -468,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +573,7 @@
         <v>40245</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -584,19 +581,19 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2">
         <v>40246</v>
       </c>
       <c r="G5" s="2">
-        <v>40246</v>
+        <v>40255</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -604,16 +601,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2">
         <v>40247</v>
@@ -627,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -636,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2">
         <v>40251</v>

</xml_diff>

<commit_message>
Small changes as per the feedback from Shannon and Tino. Update the bugs and todo list with request features.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -112,51 +111,44 @@
     <t>Creating PDFs causes application to lock until complete</t>
   </si>
   <si>
-    <t>When creating a PDF from the document viewer, the entire application will lock up and stop repainting itself until the PDF is completely built and opened. This doesn't look of feel very polished.</t>
+    <t>Switching companies sometimes doesn't update the job list</t>
+  </si>
+  <si>
+    <t>When creating a PDF from the document viewer, the entire application will lock up and stop repainting itself until the PDF is completely built and opened. This doesn't look of feel very polished. [FIX: the PDF application now runs a background thread and a message windows is now opened to indicated what is happening]</t>
+  </si>
+  <si>
+    <t>Jobs -&gt; Job List</t>
+  </si>
+  <si>
+    <t>To reproduce, make sure a job already exist in the system and used the "go to job" shortcut to get to it, then change companies and watch as the job list doesn't update.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="YYYY\-MM\-DD;@" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="SimSun"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,7 +160,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -176,81 +168,344 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.1725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.0745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="64.2313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="17.0039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.57254901960784"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="39.125" style="1"/>
+    <col min="3" max="3" width="15.25" style="1"/>
+    <col min="4" max="4" width="26.125" style="1"/>
+    <col min="5" max="5" width="64.25" style="1"/>
+    <col min="6" max="6" width="18.5" style="2"/>
+    <col min="7" max="7" width="17" style="2"/>
+    <col min="8" max="1025" width="9.625"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="5">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -273,8 +528,8 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -289,15 +544,15 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>40245</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>40245</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -312,15 +567,15 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <v>40245</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2">
         <v>40252</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -335,15 +590,15 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <v>40245</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="2">
         <v>40245</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="55.2" outlineLevel="0" r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -358,15 +613,15 @@
       <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <v>40246</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="2">
         <v>40255</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -381,15 +636,15 @@
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <v>40247</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="2">
         <v>40252</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -404,15 +659,15 @@
       <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>40251</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="2">
         <v>40252</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="82.05" outlineLevel="0" r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -427,93 +682,93 @@
       <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <v>40258</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>40258</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2">
+        <v>40257</v>
+      </c>
+      <c r="G9" s="2">
+        <v>40260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="2">
         <v>40262</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>40258</v>
+      <c r="G10" s="2">
+        <v>40262</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57254901960784"/>
+    <col min="1" max="1025" width="9.625"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57254901960784"/>
+    <col min="1" max="1025" width="9.625"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added reference numbers to jobs.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>To reproduce, make sure a job already exist in the system and used the "go to job" shortcut to get to it, then change companies and watch as the job list doesn't update.</t>
+  </si>
+  <si>
+    <t>Remove button always disabled for Loads</t>
+  </si>
+  <si>
+    <t>Jobs -&gt; Loads</t>
+  </si>
+  <si>
+    <t>There is currently no way to remove a load from a job as the remove button is always disabled.</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -735,6 +744,29 @@
         <v>40262</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="2">
+        <v>40266</v>
+      </c>
+      <c r="G11" s="2">
+        <v>40266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -747,7 +779,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="9.625"/>
   </cols>
@@ -763,7 +795,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="9.625"/>
   </cols>

</xml_diff>

<commit_message>
Fixed bugs where changing companies wouldn't update the quote or job lists.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -729,7 +729,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>33</v>
@@ -741,7 +741,7 @@
         <v>40262</v>
       </c>
       <c r="G10" s="2">
-        <v>40262</v>
+        <v>40266</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
The remove button on the loads page now actually works.
</commit_message>
<xml_diff>
--- a/Documents/Bugs.xlsx
+++ b/Documents/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>There is currently no way to remove a load from a job as the remove button is always disabled.</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Deleting a job with invoices throws an exception</t>
+  </si>
+  <si>
+    <t>If a job has any invoices associated with it and the user attempts to delete it an expeption is thrown and reported. A more friendly error message would be better.</t>
   </si>
 </sst>
 </file>
@@ -496,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -752,7 +761,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>36</v>
@@ -764,6 +773,29 @@
         <v>40266</v>
       </c>
       <c r="G11" s="2">
+        <v>40266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2">
+        <v>40266</v>
+      </c>
+      <c r="G12" s="2">
         <v>40266</v>
       </c>
     </row>

</xml_diff>